<commit_message>
More pollen tube files
</commit_message>
<xml_diff>
--- a/pollentube2021/OP9/OP9Dall_NEW.xlsx
+++ b/pollentube2021/OP9/OP9Dall_NEW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\pollentube2021\OP9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF871570-D0BA-47E9-88F0-0C0CB58D1895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B459ECFB-328A-454E-8CC0-2E066F8B7790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12888" yWindow="852" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3700,7 +3700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0998F861-211D-4DA0-B001-1C5699BC6828}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>

</xml_diff>